<commit_message>
update to allow data generators
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-outbreak-intersectional-dict.xlsx
+++ b/inst/extdata/MSF-outbreak-intersectional-dict.xlsx
@@ -266,6 +266,9 @@
     <t>Year</t>
   </si>
   <si>
+    <t>yn</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -483,9 +486,6 @@
   </si>
   <si>
     <t>Refugee</t>
-  </si>
-  <si>
-    <t>yn</t>
   </si>
   <si>
     <t xml:space="preserve">Not done</t>
@@ -3533,10 +3533,10 @@
         <v>211</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
@@ -3544,10 +3544,10 @@
         <v>211</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12">
@@ -3555,10 +3555,10 @@
         <v>211</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13">
@@ -3566,10 +3566,10 @@
         <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
@@ -3621,10 +3621,10 @@
         <v>217</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
@@ -3654,10 +3654,10 @@
         <v>220</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22">
@@ -3764,10 +3764,10 @@
         <v>248</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
@@ -3885,10 +3885,10 @@
         <v>231</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3916,16 +3916,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
@@ -4170,7 +4170,7 @@
         <v>177</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
@@ -4935,10 +4935,10 @@
         <v>177</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -4947,10 +4947,10 @@
         <v>177</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -5043,10 +5043,10 @@
         <v>268</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -5103,10 +5103,10 @@
         <v>270</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -5115,10 +5115,10 @@
         <v>272</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -5127,10 +5127,10 @@
         <v>272</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -5151,10 +5151,10 @@
         <v>272</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -5271,10 +5271,10 @@
         <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -5303,16 +5303,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
@@ -5332,7 +5332,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -5416,35 +5416,35 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
@@ -5452,10 +5452,10 @@
         <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
@@ -5463,10 +5463,10 @@
         <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
@@ -5474,10 +5474,10 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
@@ -5485,10 +5485,10 @@
         <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
@@ -5496,10 +5496,10 @@
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15">
@@ -5507,10 +5507,10 @@
         <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16">
@@ -5518,10 +5518,10 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -5529,10 +5529,10 @@
         <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -5540,10 +5540,10 @@
         <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -5551,10 +5551,10 @@
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20">
@@ -5562,10 +5562,10 @@
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -5628,10 +5628,10 @@
         <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
@@ -5639,10 +5639,10 @@
         <v>65</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
@@ -5650,10 +5650,10 @@
         <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
@@ -5661,10 +5661,10 @@
         <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30">
@@ -5672,10 +5672,10 @@
         <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31">
@@ -5683,10 +5683,10 @@
         <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32">
@@ -5694,10 +5694,10 @@
         <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
@@ -5705,10 +5705,10 @@
         <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34">
@@ -5716,10 +5716,10 @@
         <v>71</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35">
@@ -5727,10 +5727,10 @@
         <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36">
@@ -5738,10 +5738,10 @@
         <v>68</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37">
@@ -5749,10 +5749,10 @@
         <v>68</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38">
@@ -5760,10 +5760,10 @@
         <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39">
@@ -5771,10 +5771,10 @@
         <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40">
@@ -5782,10 +5782,10 @@
         <v>68</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5813,16 +5813,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
@@ -5925,10 +5925,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -5945,7 +5945,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -6062,13 +6062,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
@@ -6105,7 +6105,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
@@ -6125,10 +6125,10 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
@@ -6145,10 +6145,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
@@ -6165,10 +6165,10 @@
         <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
@@ -6185,10 +6185,10 @@
         <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
@@ -6205,10 +6205,10 @@
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
@@ -6222,10 +6222,10 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>51</v>
@@ -6242,13 +6242,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
@@ -6262,13 +6262,13 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
@@ -6285,10 +6285,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
@@ -6302,13 +6302,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
@@ -6322,13 +6322,13 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
@@ -6342,13 +6342,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -6365,10 +6365,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
@@ -6388,7 +6388,7 @@
         <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
@@ -6405,7 +6405,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>63</v>
@@ -6930,159 +6930,159 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D14" s="5"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" s="5"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>153</v>
@@ -7094,43 +7094,43 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>154</v>
@@ -7142,13 +7142,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -7169,10 +7169,10 @@
         <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="5"/>
     </row>
@@ -7205,16 +7205,16 @@
         <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>158</v>
@@ -7225,7 +7225,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>159</v>
@@ -7236,7 +7236,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>160</v>
@@ -7247,7 +7247,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>161</v>
@@ -7258,7 +7258,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>162</v>
@@ -7269,7 +7269,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>163</v>
@@ -7280,7 +7280,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>164</v>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>165</v>
@@ -7302,7 +7302,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>166</v>
@@ -7313,7 +7313,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>167</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>168</v>
@@ -7335,18 +7335,18 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>169</v>
@@ -7357,7 +7357,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>153</v>
@@ -7368,7 +7368,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>170</v>
@@ -7379,7 +7379,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>158</v>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>171</v>
@@ -7401,7 +7401,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>160</v>
@@ -7412,7 +7412,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>161</v>
@@ -7423,7 +7423,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>172</v>
@@ -7434,7 +7434,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>164</v>
@@ -7445,7 +7445,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>165</v>
@@ -7456,7 +7456,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>173</v>
@@ -7467,7 +7467,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>166</v>
@@ -7478,7 +7478,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>174</v>
@@ -7489,7 +7489,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>168</v>
@@ -7500,7 +7500,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>153</v>
@@ -7511,13 +7511,13 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -7545,16 +7545,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
@@ -7656,7 +7656,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>175</v>
@@ -8597,10 +8597,10 @@
         <v>194</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -8633,10 +8633,10 @@
         <v>194</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -8681,10 +8681,10 @@
         <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -8693,33 +8693,33 @@
         <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -8727,10 +8727,10 @@
         <v>200</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -8738,10 +8738,10 @@
         <v>200</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -8749,10 +8749,10 @@
         <v>200</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21">
@@ -8760,10 +8760,10 @@
         <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
@@ -8771,10 +8771,10 @@
         <v>188</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -8782,10 +8782,10 @@
         <v>188</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
@@ -8824,16 +8824,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
update disease specific data generation
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-outbreak-intersectional-dict.xlsx
+++ b/inst/extdata/MSF-outbreak-intersectional-dict.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria" sheetId="1" state="visible" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
   <si>
     <t>type</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cholera PCR test result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one exit_status</t>
   </si>
   <si>
     <t>exit_status</t>
@@ -2838,10 +2841,10 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>67</v>
+        <v>231</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>69</v>
@@ -2861,7 +2864,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>63</v>
@@ -3442,10 +3445,10 @@
         <v>202</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -3454,10 +3457,10 @@
         <v>202</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -3466,10 +3469,10 @@
         <v>202</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -3577,10 +3580,10 @@
         <v>211</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15">
@@ -3588,10 +3591,10 @@
         <v>217</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16">
@@ -3599,10 +3602,10 @@
         <v>217</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17">
@@ -3610,10 +3613,10 @@
         <v>217</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18">
@@ -3632,10 +3635,10 @@
         <v>220</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20">
@@ -3643,10 +3646,10 @@
         <v>220</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21">
@@ -3665,10 +3668,10 @@
         <v>220</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
@@ -3679,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24">
@@ -3690,7 +3693,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25">
@@ -3701,7 +3704,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26">
@@ -3709,59 +3712,59 @@
         <v>223</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>94</v>
@@ -3772,7 +3775,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>169</v>
@@ -3783,106 +3786,106 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>82</v>
@@ -4164,7 +4167,7 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>177</v>
@@ -4224,13 +4227,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
@@ -4244,10 +4247,10 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>221</v>
@@ -4264,10 +4267,10 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>61</v>
@@ -4284,13 +4287,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
@@ -4923,10 +4926,10 @@
         <v>177</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -4959,10 +4962,10 @@
         <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -4971,76 +4974,76 @@
         <v>177</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>81</v>
@@ -5052,55 +5055,55 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>92</v>
@@ -5112,7 +5115,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>93</v>
@@ -5124,7 +5127,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>94</v>
@@ -5136,19 +5139,19 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>82</v>
@@ -5160,13 +5163,13 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -5175,10 +5178,10 @@
         <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -5187,10 +5190,10 @@
         <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -5199,10 +5202,10 @@
         <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -5211,10 +5214,10 @@
         <v>68</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -5223,10 +5226,10 @@
         <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -5235,10 +5238,10 @@
         <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D33" s="1"/>
     </row>
@@ -5247,10 +5250,10 @@
         <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D34" s="1"/>
     </row>
@@ -5259,10 +5262,10 @@
         <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D35" s="1"/>
     </row>

</xml_diff>